<commit_message>
update pictures based on new findings from development phase
</commit_message>
<xml_diff>
--- a/03_Figures/07_Suggestion/ChartExamples.xlsx
+++ b/03_Figures/07_Suggestion/ChartExamples.xlsx
@@ -1,26 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klingo/Dropbox/Studium/(4) 2016 - Fruehlingssemester/MTRP_VirtualReality/LaTeX-Files/03_Figures/07_Suggestion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Studium\(4) 2016 - Fruehlingssemester\MTRP_VirtualReality\LaTeX-Files\03_Figures\07_Suggestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="15465" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Year Overview" sheetId="1" r:id="rId1"/>
     <sheet name="Month Overview" sheetId="2" r:id="rId2"/>
     <sheet name="MonthYear Picker" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -29,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>Month</t>
   </si>
@@ -216,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -231,13 +228,19 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -247,6 +250,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -297,6 +303,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -322,7 +329,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -408,40 +415,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>4000.0</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4400.0</c:v>
+                  <c:v>4400</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4400.0</c:v>
+                  <c:v>4400</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3800.0</c:v>
+                  <c:v>3800</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4200.0</c:v>
+                  <c:v>4200</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4400.0</c:v>
+                  <c:v>4400</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4300.0</c:v>
+                  <c:v>4300</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4400.0</c:v>
+                  <c:v>4400</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3900.0</c:v>
+                  <c:v>3900</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4400.0</c:v>
+                  <c:v>4400</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4400.0</c:v>
+                  <c:v>4400</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4400.0</c:v>
+                  <c:v>4400</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -522,40 +529,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>600.0</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>200.0</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>500.0</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>300.0</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -571,11 +578,11 @@
         </c:dLbls>
         <c:gapWidth val="32"/>
         <c:overlap val="100"/>
-        <c:axId val="1961770944"/>
-        <c:axId val="1961775680"/>
+        <c:axId val="-1715740576"/>
+        <c:axId val="-1715755808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1961770944"/>
+        <c:axId val="-1715740576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -615,10 +622,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1961775680"/>
+        <c:crossAx val="-1715755808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -626,7 +633,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1961775680"/>
+        <c:axId val="-1715755808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -646,6 +653,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -673,10 +681,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1961770944"/>
+        <c:crossAx val="-1715740576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -690,6 +698,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -715,7 +724,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -745,7 +754,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -827,7 +836,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -869,94 +878,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>47.0</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>47.0</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>74.0</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>89.0</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>89.0</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>89.0</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>145.0</c:v>
+                  <c:v>145</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>177.0</c:v>
+                  <c:v>177</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>177.0</c:v>
+                  <c:v>177</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>187.0</c:v>
+                  <c:v>187</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>187.0</c:v>
+                  <c:v>187</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>187.0</c:v>
+                  <c:v>187</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>202.0</c:v>
+                  <c:v>202</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>223.0</c:v>
+                  <c:v>223</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>240.0</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>240.0</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>295.0</c:v>
+                  <c:v>295</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>320.0</c:v>
+                  <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>320.0</c:v>
+                  <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>320.0</c:v>
+                  <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>320.0</c:v>
+                  <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>320.0</c:v>
+                  <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>320.0</c:v>
+                  <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>320.0</c:v>
+                  <c:v>320</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -993,94 +1002,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>47.0</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>59.0</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>59.0</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1096,11 +1105,11 @@
         </c:dLbls>
         <c:gapWidth val="32"/>
         <c:overlap val="100"/>
-        <c:axId val="1953652096"/>
-        <c:axId val="1953656528"/>
+        <c:axId val="-1894680848"/>
+        <c:axId val="-1894683568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1953652096"/>
+        <c:axId val="-1894680848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1140,10 +1149,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1953656528"/>
+        <c:crossAx val="-1894683568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1151,7 +1160,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1953656528"/>
+        <c:axId val="-1894683568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1171,6 +1180,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1198,10 +1208,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1953652096"/>
+        <c:crossAx val="-1894680848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1241,7 +1251,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1271,7 +1281,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2408,14 +2418,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>174624</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>174624</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2424,8 +2434,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4978400" y="2235200"/>
-          <a:ext cx="6159500" cy="0"/>
+          <a:off x="5073650" y="2158999"/>
+          <a:ext cx="6270625" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2491,13 +2501,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>734487</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>169335</xdr:rowOff>
+      <xdr:rowOff>137583</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>465667</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>169335</xdr:rowOff>
+      <xdr:rowOff>137583</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2506,8 +2516,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5687487" y="1979085"/>
-          <a:ext cx="6335180" cy="0"/>
+          <a:off x="5782737" y="1923521"/>
+          <a:ext cx="6462180" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2799,13 +2809,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView topLeftCell="D2" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2816,7 +2826,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2843,7 +2853,7 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2870,7 +2880,7 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2897,7 +2907,7 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2924,7 +2934,7 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2951,7 +2961,7 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2978,7 +2988,7 @@
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -3005,7 +3015,7 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -3032,7 +3042,7 @@
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -3059,7 +3069,7 @@
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -3086,7 +3096,7 @@
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -3113,7 +3123,7 @@
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -3140,7 +3150,7 @@
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -3153,7 +3163,7 @@
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -3173,7 +3183,7 @@
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -3186,7 +3196,7 @@
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
     </row>
-    <row r="17" spans="5:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -3199,7 +3209,7 @@
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
     </row>
-    <row r="18" spans="5:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -3212,7 +3222,7 @@
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
     </row>
-    <row r="19" spans="5:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -3225,7 +3235,7 @@
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
     </row>
-    <row r="20" spans="5:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -3238,7 +3248,7 @@
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
     </row>
-    <row r="21" spans="5:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -3251,7 +3261,7 @@
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
     </row>
-    <row r="22" spans="5:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -3264,7 +3274,7 @@
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
     </row>
-    <row r="23" spans="5:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -3277,7 +3287,7 @@
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
     </row>
-    <row r="24" spans="5:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -3290,7 +3300,7 @@
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
     </row>
-    <row r="25" spans="5:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
@@ -3303,7 +3313,7 @@
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
     </row>
-    <row r="26" spans="5:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -3316,7 +3326,7 @@
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
     </row>
-    <row r="27" spans="5:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -3329,7 +3339,7 @@
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
     </row>
-    <row r="28" spans="5:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -3342,7 +3352,7 @@
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
     </row>
-    <row r="29" spans="5:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
@@ -3355,7 +3365,7 @@
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
     </row>
-    <row r="30" spans="5:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -3382,9 +3392,9 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -3398,7 +3408,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3425,7 +3435,7 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3452,7 +3462,7 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3479,7 +3489,7 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3506,7 +3516,7 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3533,7 +3543,7 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3560,7 +3570,7 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3587,7 +3597,7 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3614,7 +3624,7 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3641,7 +3651,7 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3668,7 +3678,7 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3695,7 +3705,7 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3722,7 +3732,7 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3749,7 +3759,7 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3776,7 +3786,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3803,7 +3813,7 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3830,7 +3840,7 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3857,7 +3867,7 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3884,7 +3894,7 @@
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3911,7 +3921,7 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3938,7 +3948,7 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3965,7 +3975,7 @@
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3992,7 +4002,7 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4019,7 +4029,7 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4046,7 +4056,7 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -4073,7 +4083,7 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4100,7 +4110,7 @@
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4127,7 +4137,7 @@
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4154,7 +4164,7 @@
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4181,7 +4191,7 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4197,7 +4207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>18</v>
       </c>
@@ -4205,7 +4215,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>19</v>
       </c>
@@ -4222,18 +4232,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="8" customWidth="1"/>
+    <col min="12" max="12" width="1.375" customWidth="1"/>
+    <col min="13" max="13" width="33.25" customWidth="1"/>
+    <col min="14" max="14" width="1.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -4245,7 +4258,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -4257,23 +4270,23 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A3" s="1"/>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="6" t="s">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -4285,8 +4298,8 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" s="2" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
+    <row r="5" spans="1:15" s="2" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
       <c r="B5" s="3">
         <v>2010</v>
       </c>
@@ -4296,7 +4309,7 @@
       <c r="D5" s="3">
         <v>2012</v>
       </c>
-      <c r="E5" s="7"/>
+      <c r="E5" s="6"/>
       <c r="F5" s="3" t="s">
         <v>20</v>
       </c>
@@ -4306,11 +4319,11 @@
       <c r="H5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-    </row>
-    <row r="6" spans="1:10" s="2" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" spans="1:15" s="2" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
       <c r="B6" s="3">
         <v>2013</v>
       </c>
@@ -4320,7 +4333,7 @@
       <c r="D6" s="3">
         <v>2015</v>
       </c>
-      <c r="E6" s="7"/>
+      <c r="E6" s="6"/>
       <c r="F6" s="3" t="s">
         <v>23</v>
       </c>
@@ -4330,17 +4343,17 @@
       <c r="H6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-    </row>
-    <row r="7" spans="1:10" s="2" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="1:15" s="2" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
       <c r="B7" s="5">
         <v>2016</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="7"/>
+      <c r="E7" s="6"/>
       <c r="F7" s="3" t="s">
         <v>25</v>
       </c>
@@ -4350,15 +4363,15 @@
       <c r="H7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-    </row>
-    <row r="8" spans="1:10" s="2" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:15" s="2" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="7"/>
+      <c r="E8" s="6"/>
       <c r="F8" s="4" t="s">
         <v>28</v>
       </c>
@@ -4368,10 +4381,10 @@
       <c r="H8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -4383,7 +4396,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -4395,7 +4408,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -4407,7 +4420,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -4419,11 +4432,125 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+    </row>
+    <row r="16" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+    </row>
+    <row r="17" spans="11:15" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="5">
+        <v>2016</v>
+      </c>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+    </row>
+    <row r="18" spans="11:15" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="11:15" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="3">
+        <v>2015</v>
+      </c>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+    </row>
+    <row r="20" spans="11:15" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+    </row>
+    <row r="21" spans="11:15" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="3">
+        <v>2014</v>
+      </c>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+    </row>
+    <row r="22" spans="11:15" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+    </row>
+    <row r="23" spans="11:15" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="3">
+        <v>2013</v>
+      </c>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+    </row>
+    <row r="24" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+    </row>
+    <row r="25" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+    </row>
+    <row r="26" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+    </row>
+    <row r="27" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="F3:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>